<commit_message>
Add Power flow and print file
</commit_message>
<xml_diff>
--- a/Model_optimization/Lines_34.xlsx
+++ b/Model_optimization/Lines_34.xlsx
@@ -389,13 +389,13 @@
         <v>2</v>
       </c>
       <c r="C2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D2">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D2">
-        <v>4.8000000000000001E-2</v>
-      </c>
       <c r="E2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -412,7 +412,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -429,7 +429,7 @@
         <v>4.5699999999999998E-2</v>
       </c>
       <c r="E4">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -446,7 +446,7 @@
         <v>4.1500000000000002E-2</v>
       </c>
       <c r="E5">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>4.1500000000000002E-2</v>
       </c>
       <c r="E6">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="E7">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="E9">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E10">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E12">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E13">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E14">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E15">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E16">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>4.9799999999999997E-2</v>
       </c>
       <c r="E17">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>4.5699999999999998E-2</v>
       </c>
       <c r="E18">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>4.7300000000000002E-2</v>
       </c>
       <c r="E19">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E20">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E21">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E22">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E23">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="E24">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E25">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="E26">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E27">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E28">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E29">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E30">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E31">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E32">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="E33">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="E34">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>